<commit_message>
+ ap, cp1, cp2 and add nonce challenge
</commit_message>
<xml_diff>
--- a/src/assignment2/plots.xlsx
+++ b/src/assignment2/plots.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ISTD\ISTD\Term5\50-005\Week13\assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaojie/Work/java/cse/src/assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACCB5A0C-D1C2-48A5-B169-A28E3CA0BE63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{381B6505-BC57-4DAE-879F-211FFCFD5D32}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,18 +30,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>MODE1</t>
   </si>
   <si>
     <t>MODE2</t>
   </si>
+  <si>
+    <t>Time(ms)</t>
+  </si>
+  <si>
+    <t>Size(mb)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,7 +97,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -130,6 +141,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -194,33 +206,33 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>76944.388741000002</c:v>
+                  <c:v>76944.388741</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70490.047999999995</c:v>
+                  <c:v>70490.048</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61625.959505999999</c:v>
+                  <c:v>61625.959506</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52851.211456999998</c:v>
+                  <c:v>52851.211457</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46824.461826999999</c:v>
+                  <c:v>46824.461827</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38072.848593000002</c:v>
+                  <c:v>38072.848593</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29510.351406999998</c:v>
+                  <c:v>29510.351407</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22215.407407999999</c:v>
+                  <c:v>22215.407408</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>15518.856296</c:v>
@@ -233,45 +245,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D8E7-4BF5-A7D0-AD5401013083}"/>
             </c:ext>
@@ -306,84 +318,84 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$C$23</c:f>
+              <c:f>Sheet1!$C$16:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4066.5149630000001</c:v>
+                  <c:v>4066.514963</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3127.8802959999998</c:v>
+                  <c:v>3127.880296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2878.9127899999999</c:v>
+                  <c:v>2878.91279</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3231.64642</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3700.3117040000002</c:v>
+                  <c:v>3700.311704</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2732.123259</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2729.5217779999998</c:v>
+                  <c:v>2729.521778</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2355.2458270000002</c:v>
+                  <c:v>2355.245827</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1945.94805</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1303.7530870000001</c:v>
+                  <c:v>1303.753087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$23</c:f>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D8E7-4BF5-A7D0-AD5401013083}"/>
             </c:ext>
@@ -397,11 +409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539993704"/>
-        <c:axId val="539994032"/>
+        <c:axId val="1346821008"/>
+        <c:axId val="1346823488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539993704"/>
+        <c:axId val="1346821008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,12 +470,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539994032"/>
+        <c:crossAx val="1346823488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539994032"/>
+        <c:axId val="1346823488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539993704"/>
+        <c:crossAx val="1346821008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -534,14 +546,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1138,13 +1150,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1152,7 +1164,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9C620D-F6CD-44BC-B9E5-1B28EC9A66AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C9C620D-F6CD-44BC-B9E5-1B28EC9A66AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1469,182 +1481,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3868771-5065-4225-A6F9-20F508FB09DF}">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>76944.388741000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>70490.047999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>61625.959505999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>52851.211456999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>46824.461826999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>38072.848593000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>29510.351406999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>22215.407407999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>15518.856296</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>6848.768</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>4066.5149630000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>9</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>3127.8802959999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>8</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <v>2878.9127899999999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>7</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>3231.64642</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>6</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>3700.3117040000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>5</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>2732.123259</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>2729.5217779999998</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>3</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>2355.2458270000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>2</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>1945.94805</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>1303.7530870000001</v>
       </c>
     </row>

</xml_diff>